<commit_message>
Ajout N°secu et quelques création de patient en plus
</commit_message>
<xml_diff>
--- a/docs/tableaux/tableauPatient.xlsx
+++ b/docs/tableaux/tableauPatient.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22624"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22730"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\aurel\Desktop\sweatcare\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\git-repos\cda-pfr-projet-fil-rouge-sante\docs\tableaux\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{03A5F618-640D-4920-9179-3E2A21B26A94}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{837B4834-11F8-4840-AA9E-8F13C3DB5CE1}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5700" yWindow="285" windowWidth="13080" windowHeight="11400" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="24240" windowHeight="13140" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="223" uniqueCount="147">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="430" uniqueCount="269">
   <si>
     <t>idPatient</t>
   </si>
@@ -465,7 +465,373 @@
     <t>09 12 22 08 34</t>
   </si>
   <si>
-    <t>09 2 22 08 34</t>
+    <t>09 87 52 63 33</t>
+  </si>
+  <si>
+    <t>06 45 65 98 98</t>
+  </si>
+  <si>
+    <t>03 20 50 40 40</t>
+  </si>
+  <si>
+    <t xml:space="preserve">03 21 30 30 21 </t>
+  </si>
+  <si>
+    <t>03 20 30 20 03</t>
+  </si>
+  <si>
+    <t>03 21 21 30 21</t>
+  </si>
+  <si>
+    <t>03 32 35 84 84</t>
+  </si>
+  <si>
+    <t xml:space="preserve">03 23 32 10 51 </t>
+  </si>
+  <si>
+    <t>03 21 21 87 89</t>
+  </si>
+  <si>
+    <t>09 02 22 08 34</t>
+  </si>
+  <si>
+    <t>03 20 20 20 20</t>
+  </si>
+  <si>
+    <t>03 21 11 22 33</t>
+  </si>
+  <si>
+    <t>03 21 88 88 99</t>
+  </si>
+  <si>
+    <t>03 20 22 55 88</t>
+  </si>
+  <si>
+    <t>09 10 56 98 33</t>
+  </si>
+  <si>
+    <t>09 80 51 23 44</t>
+  </si>
+  <si>
+    <t>09 87 65 32 15</t>
+  </si>
+  <si>
+    <t>09 78 98 78 98</t>
+  </si>
+  <si>
+    <t>09 23 65 98 15</t>
+  </si>
+  <si>
+    <t xml:space="preserve">09 88 98 98 65 </t>
+  </si>
+  <si>
+    <t>03 20 21 21 60</t>
+  </si>
+  <si>
+    <t>09 89 63 36 65</t>
+  </si>
+  <si>
+    <t>09 56 65 98 12</t>
+  </si>
+  <si>
+    <t>03 23 23 84 89</t>
+  </si>
+  <si>
+    <t>03 20 20 99 99</t>
+  </si>
+  <si>
+    <t>03 21 87 87 87</t>
+  </si>
+  <si>
+    <t>03 56 56 45 45</t>
+  </si>
+  <si>
+    <t xml:space="preserve">03 21 65 98 89 </t>
+  </si>
+  <si>
+    <t>03 56 89 54 54</t>
+  </si>
+  <si>
+    <t>09 87 89 32 23</t>
+  </si>
+  <si>
+    <t>09 87 87 89 98</t>
+  </si>
+  <si>
+    <t>09 23 56 65 56</t>
+  </si>
+  <si>
+    <t>03 23 65 65 23</t>
+  </si>
+  <si>
+    <t>03 21 21 23 88</t>
+  </si>
+  <si>
+    <t>03 21 66 44 77</t>
+  </si>
+  <si>
+    <t>03 55 55 88 88</t>
+  </si>
+  <si>
+    <t>03 23 98 89 77</t>
+  </si>
+  <si>
+    <t>03 45 65 56 65</t>
+  </si>
+  <si>
+    <t>03 21 11 44 77</t>
+  </si>
+  <si>
+    <t>54 Rue des oiseaux</t>
+  </si>
+  <si>
+    <t>1b place de l'église</t>
+  </si>
+  <si>
+    <t>37 Rue de Tourcoing</t>
+  </si>
+  <si>
+    <t>12 Rue Gambetta</t>
+  </si>
+  <si>
+    <t>23 Place de la monnaie</t>
+  </si>
+  <si>
+    <t>32 Faubourg Jean Jaurès</t>
+  </si>
+  <si>
+    <t>135 Rue Nationale</t>
+  </si>
+  <si>
+    <t>77  Rue Jules Guesde</t>
+  </si>
+  <si>
+    <t>26 Rue Solférino</t>
+  </si>
+  <si>
+    <t>23 Grand Place</t>
+  </si>
+  <si>
+    <t>65 Rue de la soif</t>
+  </si>
+  <si>
+    <t>32 Rue de la soif</t>
+  </si>
+  <si>
+    <t>3 Rue Solférino, Apt25</t>
+  </si>
+  <si>
+    <t>32 Rue de Gand</t>
+  </si>
+  <si>
+    <t>44 Rue de Gand</t>
+  </si>
+  <si>
+    <t>23 Rue Nationale</t>
+  </si>
+  <si>
+    <t>192 Rue Nationale</t>
+  </si>
+  <si>
+    <t>70 Rue du Général de Gaulles</t>
+  </si>
+  <si>
+    <t>25 Rue du Général Leclerc</t>
+  </si>
+  <si>
+    <t>19 Rue de la monnaie</t>
+  </si>
+  <si>
+    <t>31 Rue de l'école</t>
+  </si>
+  <si>
+    <t>65 Rue de Roubaix</t>
+  </si>
+  <si>
+    <t>137 Rue de Tourcoing</t>
+  </si>
+  <si>
+    <t>26 Allée des sages</t>
+  </si>
+  <si>
+    <t>25 Boulevard Excellemans</t>
+  </si>
+  <si>
+    <t>30 Rue Solférino</t>
+  </si>
+  <si>
+    <t>91 Rue Nationale, apt24</t>
+  </si>
+  <si>
+    <t>149 Rue du Général de Gaulles</t>
+  </si>
+  <si>
+    <t>2 Rue de la Monnaie</t>
+  </si>
+  <si>
+    <t>LEROY</t>
+  </si>
+  <si>
+    <t>Timothé</t>
+  </si>
+  <si>
+    <t>DURAND</t>
+  </si>
+  <si>
+    <t>Laura</t>
+  </si>
+  <si>
+    <t>MENDEZ</t>
+  </si>
+  <si>
+    <t>Alicia</t>
+  </si>
+  <si>
+    <t>BARGUI</t>
+  </si>
+  <si>
+    <t>Mohamed</t>
+  </si>
+  <si>
+    <t>N'GUYEN</t>
+  </si>
+  <si>
+    <t>Tao</t>
+  </si>
+  <si>
+    <t>Virginie</t>
+  </si>
+  <si>
+    <t>DETEZ</t>
+  </si>
+  <si>
+    <t>DEWAHIE</t>
+  </si>
+  <si>
+    <t>Téo</t>
+  </si>
+  <si>
+    <t>PETIT</t>
+  </si>
+  <si>
+    <t>Carine</t>
+  </si>
+  <si>
+    <t>SALUN</t>
+  </si>
+  <si>
+    <t>Stéphanie</t>
+  </si>
+  <si>
+    <t>SUAREZ</t>
+  </si>
+  <si>
+    <t>Arthuro</t>
+  </si>
+  <si>
+    <t>VAN BERGUER</t>
+  </si>
+  <si>
+    <t>Fanny</t>
+  </si>
+  <si>
+    <t>HERTEM</t>
+  </si>
+  <si>
+    <t>Téa</t>
+  </si>
+  <si>
+    <t>ALDON</t>
+  </si>
+  <si>
+    <t>Frédéric</t>
+  </si>
+  <si>
+    <t>Marion</t>
+  </si>
+  <si>
+    <t>Thibault</t>
+  </si>
+  <si>
+    <t>Marie</t>
+  </si>
+  <si>
+    <t>Corentin</t>
+  </si>
+  <si>
+    <t>Albert</t>
+  </si>
+  <si>
+    <t>Stéphane</t>
+  </si>
+  <si>
+    <t>Camille</t>
+  </si>
+  <si>
+    <t>Alice</t>
+  </si>
+  <si>
+    <t>Paul</t>
+  </si>
+  <si>
+    <t>Gabin</t>
+  </si>
+  <si>
+    <t>TOURU</t>
+  </si>
+  <si>
+    <t>BONDRIT</t>
+  </si>
+  <si>
+    <t>POURTOI</t>
+  </si>
+  <si>
+    <t>MULLIER</t>
+  </si>
+  <si>
+    <t>FOURNIER</t>
+  </si>
+  <si>
+    <t>SAGE</t>
+  </si>
+  <si>
+    <t>PARRAIN</t>
+  </si>
+  <si>
+    <t>LUCAS</t>
+  </si>
+  <si>
+    <t>MONDON</t>
+  </si>
+  <si>
+    <t>CUEILLE</t>
+  </si>
+  <si>
+    <t>COGNARD</t>
+  </si>
+  <si>
+    <t>MORLIERE</t>
+  </si>
+  <si>
+    <t>TREUILLARD</t>
+  </si>
+  <si>
+    <t>BADRAN</t>
+  </si>
+  <si>
+    <t>TRUSSANT</t>
+  </si>
+  <si>
+    <t>GIBOURI</t>
+  </si>
+  <si>
+    <t>TRANCHANT</t>
+  </si>
+  <si>
+    <t>FILLOT</t>
+  </si>
+  <si>
+    <t>DELAUME</t>
   </si>
 </sst>
 </file>
@@ -784,10 +1150,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:J38"/>
+  <dimension ref="A1:J71"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="F16" workbookViewId="0">
-      <selection activeCell="J37" sqref="J37"/>
+    <sheetView tabSelected="1" topLeftCell="A46" workbookViewId="0">
+      <selection activeCell="B71" sqref="B71"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -839,6 +1205,9 @@
       <c r="A2">
         <v>1</v>
       </c>
+      <c r="B2">
+        <v>181025900000001</v>
+      </c>
       <c r="C2" t="s">
         <v>5</v>
       </c>
@@ -868,6 +1237,9 @@
       <c r="A3">
         <v>2</v>
       </c>
+      <c r="B3">
+        <v>280055900000002</v>
+      </c>
       <c r="C3" t="s">
         <v>5</v>
       </c>
@@ -897,6 +1269,9 @@
       <c r="A4">
         <v>3</v>
       </c>
+      <c r="B4">
+        <v>111115900000003</v>
+      </c>
       <c r="C4" t="s">
         <v>5</v>
       </c>
@@ -926,6 +1301,9 @@
       <c r="A5">
         <v>4</v>
       </c>
+      <c r="B5">
+        <v>164126200000004</v>
+      </c>
       <c r="C5" t="s">
         <v>6</v>
       </c>
@@ -955,6 +1333,9 @@
       <c r="A6">
         <v>5</v>
       </c>
+      <c r="B6">
+        <v>297110300000005</v>
+      </c>
       <c r="C6" t="s">
         <v>7</v>
       </c>
@@ -984,6 +1365,9 @@
       <c r="A7">
         <v>6</v>
       </c>
+      <c r="B7">
+        <v>176076200000006</v>
+      </c>
       <c r="C7" t="s">
         <v>8</v>
       </c>
@@ -1013,6 +1397,9 @@
       <c r="A8">
         <v>7</v>
       </c>
+      <c r="B8">
+        <v>286015900000007</v>
+      </c>
       <c r="C8" t="s">
         <v>6</v>
       </c>
@@ -1042,6 +1429,9 @@
       <c r="A9">
         <v>8</v>
       </c>
+      <c r="B9">
+        <v>202098100000008</v>
+      </c>
       <c r="C9" t="s">
         <v>9</v>
       </c>
@@ -1071,6 +1461,9 @@
       <c r="A10">
         <v>9</v>
       </c>
+      <c r="B10">
+        <v>194037600000009</v>
+      </c>
       <c r="C10" t="s">
         <v>10</v>
       </c>
@@ -1100,6 +1493,9 @@
       <c r="A11">
         <v>10</v>
       </c>
+      <c r="B11">
+        <v>153025900000010</v>
+      </c>
       <c r="C11" t="s">
         <v>11</v>
       </c>
@@ -1129,6 +1525,9 @@
       <c r="A12">
         <v>11</v>
       </c>
+      <c r="B12">
+        <v>196016200000011</v>
+      </c>
       <c r="C12" t="s">
         <v>12</v>
       </c>
@@ -1158,6 +1557,9 @@
       <c r="A13">
         <v>12</v>
       </c>
+      <c r="B13">
+        <v>182045900000012</v>
+      </c>
       <c r="C13" t="s">
         <v>13</v>
       </c>
@@ -1187,6 +1589,9 @@
       <c r="A14">
         <v>13</v>
       </c>
+      <c r="B14">
+        <v>207105900000013</v>
+      </c>
       <c r="C14" t="s">
         <v>14</v>
       </c>
@@ -1216,6 +1621,9 @@
       <c r="A15">
         <v>14</v>
       </c>
+      <c r="B15">
+        <v>280094400000014</v>
+      </c>
       <c r="C15" t="s">
         <v>14</v>
       </c>
@@ -1245,6 +1653,9 @@
       <c r="A16">
         <v>15</v>
       </c>
+      <c r="B16">
+        <v>178035900000015</v>
+      </c>
       <c r="C16" t="s">
         <v>15</v>
       </c>
@@ -1274,6 +1685,9 @@
       <c r="A17">
         <v>16</v>
       </c>
+      <c r="B17">
+        <v>281086200000016</v>
+      </c>
       <c r="C17" t="s">
         <v>16</v>
       </c>
@@ -1303,6 +1717,9 @@
       <c r="A18">
         <v>17</v>
       </c>
+      <c r="B18">
+        <v>208085900000017</v>
+      </c>
       <c r="C18" t="s">
         <v>17</v>
       </c>
@@ -1332,6 +1749,9 @@
       <c r="A19">
         <v>18</v>
       </c>
+      <c r="B19">
+        <v>113035900000018</v>
+      </c>
       <c r="C19" t="s">
         <v>18</v>
       </c>
@@ -1361,6 +1781,9 @@
       <c r="A20">
         <v>19</v>
       </c>
+      <c r="B20">
+        <v>192105900000019</v>
+      </c>
       <c r="C20" t="s">
         <v>19</v>
       </c>
@@ -1390,6 +1813,9 @@
       <c r="A21">
         <v>20</v>
       </c>
+      <c r="B21">
+        <v>166025900000020</v>
+      </c>
       <c r="C21" t="s">
         <v>20</v>
       </c>
@@ -1419,6 +1845,9 @@
       <c r="A22">
         <v>21</v>
       </c>
+      <c r="B22">
+        <v>271123700000021</v>
+      </c>
       <c r="C22" t="s">
         <v>21</v>
       </c>
@@ -1448,6 +1877,9 @@
       <c r="A23">
         <v>22</v>
       </c>
+      <c r="B23">
+        <v>200020100000022</v>
+      </c>
       <c r="C23" t="s">
         <v>22</v>
       </c>
@@ -1477,6 +1909,9 @@
       <c r="A24">
         <v>23</v>
       </c>
+      <c r="B24">
+        <v>179035900000023</v>
+      </c>
       <c r="C24" t="s">
         <v>23</v>
       </c>
@@ -1506,6 +1941,9 @@
       <c r="A25">
         <v>24</v>
       </c>
+      <c r="B25">
+        <v>146065400000024</v>
+      </c>
       <c r="C25" t="s">
         <v>24</v>
       </c>
@@ -1535,6 +1973,9 @@
       <c r="A26">
         <v>25</v>
       </c>
+      <c r="B26">
+        <v>102045900000025</v>
+      </c>
       <c r="C26" t="s">
         <v>25</v>
       </c>
@@ -1564,6 +2005,9 @@
       <c r="A27">
         <v>26</v>
       </c>
+      <c r="B27">
+        <v>254065900000056</v>
+      </c>
       <c r="C27" t="s">
         <v>26</v>
       </c>
@@ -1593,6 +2037,9 @@
       <c r="A28">
         <v>27</v>
       </c>
+      <c r="B28">
+        <v>296096200000027</v>
+      </c>
       <c r="C28" t="s">
         <v>27</v>
       </c>
@@ -1613,12 +2060,18 @@
       </c>
       <c r="I28" t="s">
         <v>84</v>
+      </c>
+      <c r="J28" t="s">
+        <v>146</v>
       </c>
     </row>
     <row r="29" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A29">
         <v>28</v>
       </c>
+      <c r="B29">
+        <v>201015900000028</v>
+      </c>
       <c r="C29" t="s">
         <v>28</v>
       </c>
@@ -1639,12 +2092,18 @@
       </c>
       <c r="I29" t="s">
         <v>84</v>
+      </c>
+      <c r="J29" t="s">
+        <v>147</v>
       </c>
     </row>
     <row r="30" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A30">
         <v>29</v>
       </c>
+      <c r="B30">
+        <v>188065900000029</v>
+      </c>
       <c r="C30" t="s">
         <v>29</v>
       </c>
@@ -1665,12 +2124,18 @@
       </c>
       <c r="I30" t="s">
         <v>84</v>
+      </c>
+      <c r="J30" t="s">
+        <v>148</v>
       </c>
     </row>
     <row r="31" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A31">
         <v>30</v>
       </c>
+      <c r="B31">
+        <v>174075900000030</v>
+      </c>
       <c r="C31" t="s">
         <v>30</v>
       </c>
@@ -1691,12 +2156,18 @@
       </c>
       <c r="I31" t="s">
         <v>84</v>
+      </c>
+      <c r="J31" t="s">
+        <v>149</v>
       </c>
     </row>
     <row r="32" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A32">
         <v>31</v>
       </c>
+      <c r="B32">
+        <v>199126200000031</v>
+      </c>
       <c r="C32" t="s">
         <v>31</v>
       </c>
@@ -1717,12 +2188,18 @@
       </c>
       <c r="I32" t="s">
         <v>84</v>
+      </c>
+      <c r="J32" t="s">
+        <v>150</v>
       </c>
     </row>
     <row r="33" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A33">
         <v>32</v>
       </c>
+      <c r="B33">
+        <v>175115900000032</v>
+      </c>
       <c r="C33" t="s">
         <v>32</v>
       </c>
@@ -1743,12 +2220,18 @@
       </c>
       <c r="I33" t="s">
         <v>85</v>
+      </c>
+      <c r="J33" t="s">
+        <v>151</v>
       </c>
     </row>
     <row r="34" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A34">
         <v>33</v>
       </c>
+      <c r="B34">
+        <v>163055900000033</v>
+      </c>
       <c r="C34" t="s">
         <v>33</v>
       </c>
@@ -1769,12 +2252,18 @@
       </c>
       <c r="I34" t="s">
         <v>85</v>
+      </c>
+      <c r="J34" t="s">
+        <v>152</v>
       </c>
     </row>
     <row r="35" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A35">
         <v>34</v>
       </c>
+      <c r="B35">
+        <v>160095900000034</v>
+      </c>
       <c r="C35" t="s">
         <v>35</v>
       </c>
@@ -1795,12 +2284,18 @@
       </c>
       <c r="I35" t="s">
         <v>86</v>
+      </c>
+      <c r="J35" t="s">
+        <v>153</v>
       </c>
     </row>
     <row r="36" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A36">
         <v>35</v>
       </c>
+      <c r="B36">
+        <v>262015900000035</v>
+      </c>
       <c r="C36" t="s">
         <v>35</v>
       </c>
@@ -1821,12 +2316,18 @@
       </c>
       <c r="I36" t="s">
         <v>87</v>
+      </c>
+      <c r="J36" t="s">
+        <v>154</v>
       </c>
     </row>
     <row r="37" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A37">
         <v>36</v>
       </c>
+      <c r="B37">
+        <v>183047600000036</v>
+      </c>
       <c r="C37" t="s">
         <v>36</v>
       </c>
@@ -1849,13 +2350,16 @@
         <v>87</v>
       </c>
       <c r="J37" t="s">
-        <v>146</v>
+        <v>155</v>
       </c>
     </row>
     <row r="38" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A38">
         <v>37</v>
       </c>
+      <c r="B38">
+        <v>119065900000037</v>
+      </c>
       <c r="C38" t="s">
         <v>36</v>
       </c>
@@ -1879,6 +2383,1062 @@
       </c>
       <c r="J38" t="s">
         <v>145</v>
+      </c>
+    </row>
+    <row r="39" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A39">
+        <v>38</v>
+      </c>
+      <c r="B39">
+        <v>196055900000038</v>
+      </c>
+      <c r="C39" t="s">
+        <v>214</v>
+      </c>
+      <c r="D39" t="s">
+        <v>215</v>
+      </c>
+      <c r="E39" t="s">
+        <v>78</v>
+      </c>
+      <c r="F39" s="1">
+        <v>35206</v>
+      </c>
+      <c r="G39" t="s">
+        <v>185</v>
+      </c>
+      <c r="H39">
+        <v>59350</v>
+      </c>
+      <c r="I39" t="s">
+        <v>87</v>
+      </c>
+      <c r="J39" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="40" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A40">
+        <v>39</v>
+      </c>
+      <c r="B40">
+        <v>298015900000039</v>
+      </c>
+      <c r="C40" t="s">
+        <v>216</v>
+      </c>
+      <c r="D40" t="s">
+        <v>217</v>
+      </c>
+      <c r="E40" t="s">
+        <v>79</v>
+      </c>
+      <c r="F40" s="1">
+        <v>35807</v>
+      </c>
+      <c r="G40" t="s">
+        <v>185</v>
+      </c>
+      <c r="H40">
+        <v>59350</v>
+      </c>
+      <c r="I40" t="s">
+        <v>87</v>
+      </c>
+      <c r="J40" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="41" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A41">
+        <v>40</v>
+      </c>
+      <c r="B41">
+        <v>251026200000040</v>
+      </c>
+      <c r="C41" t="s">
+        <v>218</v>
+      </c>
+      <c r="D41" t="s">
+        <v>219</v>
+      </c>
+      <c r="E41" t="s">
+        <v>79</v>
+      </c>
+      <c r="F41" s="1">
+        <v>18685</v>
+      </c>
+      <c r="G41" t="s">
+        <v>186</v>
+      </c>
+      <c r="H41">
+        <v>59350</v>
+      </c>
+      <c r="I41" t="s">
+        <v>87</v>
+      </c>
+      <c r="J41" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="42" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A42">
+        <v>41</v>
+      </c>
+      <c r="B42">
+        <v>256055900000041</v>
+      </c>
+      <c r="C42" t="s">
+        <v>225</v>
+      </c>
+      <c r="D42" t="s">
+        <v>224</v>
+      </c>
+      <c r="E42" t="s">
+        <v>79</v>
+      </c>
+      <c r="F42" s="1">
+        <v>20594</v>
+      </c>
+      <c r="G42" t="s">
+        <v>187</v>
+      </c>
+      <c r="H42">
+        <v>59350</v>
+      </c>
+      <c r="I42" t="s">
+        <v>87</v>
+      </c>
+      <c r="J42" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="43" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A43">
+        <v>42</v>
+      </c>
+      <c r="B43">
+        <v>172017500000042</v>
+      </c>
+      <c r="C43" t="s">
+        <v>222</v>
+      </c>
+      <c r="D43" t="s">
+        <v>223</v>
+      </c>
+      <c r="E43" t="s">
+        <v>78</v>
+      </c>
+      <c r="F43" s="1">
+        <v>26299</v>
+      </c>
+      <c r="G43" t="s">
+        <v>188</v>
+      </c>
+      <c r="H43">
+        <v>59350</v>
+      </c>
+      <c r="I43" t="s">
+        <v>87</v>
+      </c>
+      <c r="J43" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="44" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A44">
+        <v>43</v>
+      </c>
+      <c r="B44">
+        <v>275045900000043</v>
+      </c>
+      <c r="C44" t="s">
+        <v>226</v>
+      </c>
+      <c r="D44" t="s">
+        <v>38</v>
+      </c>
+      <c r="E44" t="s">
+        <v>79</v>
+      </c>
+      <c r="F44" s="1">
+        <v>27507</v>
+      </c>
+      <c r="G44" t="s">
+        <v>188</v>
+      </c>
+      <c r="H44">
+        <v>59350</v>
+      </c>
+      <c r="I44" t="s">
+        <v>87</v>
+      </c>
+      <c r="J44" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="45" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A45">
+        <v>44</v>
+      </c>
+      <c r="B45">
+        <v>199115900000044</v>
+      </c>
+      <c r="C45" t="s">
+        <v>220</v>
+      </c>
+      <c r="D45" t="s">
+        <v>221</v>
+      </c>
+      <c r="E45" t="s">
+        <v>78</v>
+      </c>
+      <c r="F45" s="1">
+        <v>36474</v>
+      </c>
+      <c r="G45" t="s">
+        <v>188</v>
+      </c>
+      <c r="H45">
+        <v>59350</v>
+      </c>
+      <c r="I45" t="s">
+        <v>87</v>
+      </c>
+      <c r="J45" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="46" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A46">
+        <v>45</v>
+      </c>
+      <c r="B46">
+        <v>103035900000045</v>
+      </c>
+      <c r="C46" t="s">
+        <v>228</v>
+      </c>
+      <c r="D46" t="s">
+        <v>227</v>
+      </c>
+      <c r="E46" t="s">
+        <v>78</v>
+      </c>
+      <c r="F46" s="1">
+        <v>37703</v>
+      </c>
+      <c r="G46" t="s">
+        <v>188</v>
+      </c>
+      <c r="H46">
+        <v>59350</v>
+      </c>
+      <c r="I46" t="s">
+        <v>87</v>
+      </c>
+      <c r="J46" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="47" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A47">
+        <v>46</v>
+      </c>
+      <c r="B47">
+        <v>264126200000046</v>
+      </c>
+      <c r="C47" t="s">
+        <v>6</v>
+      </c>
+      <c r="D47" t="s">
+        <v>229</v>
+      </c>
+      <c r="E47" t="s">
+        <v>79</v>
+      </c>
+      <c r="F47" s="1">
+        <v>23721</v>
+      </c>
+      <c r="G47" t="s">
+        <v>189</v>
+      </c>
+      <c r="H47">
+        <v>59000</v>
+      </c>
+      <c r="I47" t="s">
+        <v>81</v>
+      </c>
+      <c r="J47" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="48" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A48">
+        <v>47</v>
+      </c>
+      <c r="B48">
+        <v>286015900000047</v>
+      </c>
+      <c r="C48" t="s">
+        <v>230</v>
+      </c>
+      <c r="D48" t="s">
+        <v>231</v>
+      </c>
+      <c r="E48" t="s">
+        <v>79</v>
+      </c>
+      <c r="F48" s="1">
+        <v>31423</v>
+      </c>
+      <c r="G48" t="s">
+        <v>190</v>
+      </c>
+      <c r="H48">
+        <v>59000</v>
+      </c>
+      <c r="I48" t="s">
+        <v>81</v>
+      </c>
+      <c r="J48" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="49" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A49">
+        <v>48</v>
+      </c>
+      <c r="B49">
+        <v>192115900000048</v>
+      </c>
+      <c r="C49" t="s">
+        <v>232</v>
+      </c>
+      <c r="D49" t="s">
+        <v>233</v>
+      </c>
+      <c r="E49" t="s">
+        <v>78</v>
+      </c>
+      <c r="F49" s="1">
+        <v>33931</v>
+      </c>
+      <c r="G49" t="s">
+        <v>191</v>
+      </c>
+      <c r="H49">
+        <v>59000</v>
+      </c>
+      <c r="I49" t="s">
+        <v>81</v>
+      </c>
+      <c r="J49" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="50" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A50">
+        <v>49</v>
+      </c>
+      <c r="B50">
+        <v>295065900000049</v>
+      </c>
+      <c r="C50" t="s">
+        <v>234</v>
+      </c>
+      <c r="D50" t="s">
+        <v>235</v>
+      </c>
+      <c r="E50" t="s">
+        <v>79</v>
+      </c>
+      <c r="F50" s="1">
+        <v>34880</v>
+      </c>
+      <c r="G50" t="s">
+        <v>192</v>
+      </c>
+      <c r="H50">
+        <v>59000</v>
+      </c>
+      <c r="I50" t="s">
+        <v>81</v>
+      </c>
+      <c r="J50" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="51" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A51">
+        <v>50</v>
+      </c>
+      <c r="B51">
+        <v>294105900000050</v>
+      </c>
+      <c r="C51" t="s">
+        <v>236</v>
+      </c>
+      <c r="D51" t="s">
+        <v>237</v>
+      </c>
+      <c r="E51" t="s">
+        <v>79</v>
+      </c>
+      <c r="F51" s="1">
+        <v>34612</v>
+      </c>
+      <c r="G51" t="s">
+        <v>193</v>
+      </c>
+      <c r="H51">
+        <v>59000</v>
+      </c>
+      <c r="I51" t="s">
+        <v>81</v>
+      </c>
+      <c r="J51" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="52" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A52">
+        <v>51</v>
+      </c>
+      <c r="B52">
+        <v>277085900000051</v>
+      </c>
+      <c r="C52" t="s">
+        <v>238</v>
+      </c>
+      <c r="D52" t="s">
+        <v>41</v>
+      </c>
+      <c r="E52" t="s">
+        <v>79</v>
+      </c>
+      <c r="F52" s="1">
+        <v>28350</v>
+      </c>
+      <c r="G52" t="s">
+        <v>194</v>
+      </c>
+      <c r="H52">
+        <v>59000</v>
+      </c>
+      <c r="I52" t="s">
+        <v>81</v>
+      </c>
+      <c r="J52" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="53" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A53">
+        <v>52</v>
+      </c>
+      <c r="B53">
+        <v>182071200000052</v>
+      </c>
+      <c r="C53" t="s">
+        <v>250</v>
+      </c>
+      <c r="D53" t="s">
+        <v>239</v>
+      </c>
+      <c r="E53" t="s">
+        <v>78</v>
+      </c>
+      <c r="F53" s="1">
+        <v>30163</v>
+      </c>
+      <c r="G53" t="s">
+        <v>195</v>
+      </c>
+      <c r="H53">
+        <v>59000</v>
+      </c>
+      <c r="I53" t="s">
+        <v>81</v>
+      </c>
+      <c r="J53" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="54" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A54">
+        <v>53</v>
+      </c>
+      <c r="B54">
+        <v>258055900000053</v>
+      </c>
+      <c r="C54" t="s">
+        <v>251</v>
+      </c>
+      <c r="D54" t="s">
+        <v>240</v>
+      </c>
+      <c r="E54" t="s">
+        <v>79</v>
+      </c>
+      <c r="F54" s="1">
+        <v>21330</v>
+      </c>
+      <c r="G54" t="s">
+        <v>196</v>
+      </c>
+      <c r="H54">
+        <v>59000</v>
+      </c>
+      <c r="I54" t="s">
+        <v>81</v>
+      </c>
+      <c r="J54" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="55" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A55">
+        <v>54</v>
+      </c>
+      <c r="B55">
+        <v>183035900000054</v>
+      </c>
+      <c r="C55" t="s">
+        <v>252</v>
+      </c>
+      <c r="D55" t="s">
+        <v>241</v>
+      </c>
+      <c r="E55" t="s">
+        <v>78</v>
+      </c>
+      <c r="F55" s="1">
+        <v>30387</v>
+      </c>
+      <c r="G55" t="s">
+        <v>197</v>
+      </c>
+      <c r="H55">
+        <v>59000</v>
+      </c>
+      <c r="I55" t="s">
+        <v>81</v>
+      </c>
+      <c r="J55" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="56" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A56">
+        <v>55</v>
+      </c>
+      <c r="B56">
+        <v>100026200000055</v>
+      </c>
+      <c r="C56" t="s">
+        <v>253</v>
+      </c>
+      <c r="D56" t="s">
+        <v>59</v>
+      </c>
+      <c r="E56" t="s">
+        <v>78</v>
+      </c>
+      <c r="F56" s="1">
+        <v>36585</v>
+      </c>
+      <c r="G56" t="s">
+        <v>198</v>
+      </c>
+      <c r="H56">
+        <v>59000</v>
+      </c>
+      <c r="I56" t="s">
+        <v>81</v>
+      </c>
+      <c r="J56" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="57" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A57">
+        <v>56</v>
+      </c>
+      <c r="B57">
+        <v>276095900000056</v>
+      </c>
+      <c r="C57" t="s">
+        <v>254</v>
+      </c>
+      <c r="D57" t="s">
+        <v>242</v>
+      </c>
+      <c r="E57" t="s">
+        <v>79</v>
+      </c>
+      <c r="F57" s="1">
+        <v>28017</v>
+      </c>
+      <c r="G57" t="s">
+        <v>199</v>
+      </c>
+      <c r="H57">
+        <v>59000</v>
+      </c>
+      <c r="I57" t="s">
+        <v>81</v>
+      </c>
+      <c r="J57" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="58" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A58">
+        <v>57</v>
+      </c>
+      <c r="B58">
+        <v>192065900000057</v>
+      </c>
+      <c r="C58" t="s">
+        <v>255</v>
+      </c>
+      <c r="D58" t="s">
+        <v>243</v>
+      </c>
+      <c r="E58" t="s">
+        <v>78</v>
+      </c>
+      <c r="F58" s="1">
+        <v>33781</v>
+      </c>
+      <c r="G58" t="s">
+        <v>200</v>
+      </c>
+      <c r="H58">
+        <v>59000</v>
+      </c>
+      <c r="I58" t="s">
+        <v>81</v>
+      </c>
+      <c r="J58" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="59" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A59">
+        <v>58</v>
+      </c>
+      <c r="B59">
+        <v>262075900000058</v>
+      </c>
+      <c r="C59" t="s">
+        <v>256</v>
+      </c>
+      <c r="D59" t="s">
+        <v>50</v>
+      </c>
+      <c r="E59" t="s">
+        <v>79</v>
+      </c>
+      <c r="F59" s="1">
+        <v>22841</v>
+      </c>
+      <c r="G59" t="s">
+        <v>201</v>
+      </c>
+      <c r="H59">
+        <v>59000</v>
+      </c>
+      <c r="I59" t="s">
+        <v>81</v>
+      </c>
+      <c r="J59" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="60" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A60">
+        <v>59</v>
+      </c>
+      <c r="B60">
+        <v>159065900000059</v>
+      </c>
+      <c r="C60" t="s">
+        <v>257</v>
+      </c>
+      <c r="D60" t="s">
+        <v>244</v>
+      </c>
+      <c r="E60" t="s">
+        <v>78</v>
+      </c>
+      <c r="F60" s="1">
+        <v>21703</v>
+      </c>
+      <c r="G60" t="s">
+        <v>202</v>
+      </c>
+      <c r="H60">
+        <v>59000</v>
+      </c>
+      <c r="I60" t="s">
+        <v>81</v>
+      </c>
+      <c r="J60" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="61" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A61">
+        <v>60</v>
+      </c>
+      <c r="B61">
+        <v>154035900000060</v>
+      </c>
+      <c r="C61" t="s">
+        <v>258</v>
+      </c>
+      <c r="D61" t="s">
+        <v>61</v>
+      </c>
+      <c r="E61" t="s">
+        <v>78</v>
+      </c>
+      <c r="F61" s="1">
+        <v>34415</v>
+      </c>
+      <c r="G61" t="s">
+        <v>203</v>
+      </c>
+      <c r="H61">
+        <v>59000</v>
+      </c>
+      <c r="I61" t="s">
+        <v>81</v>
+      </c>
+      <c r="J61" t="s">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="62" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A62">
+        <v>61</v>
+      </c>
+      <c r="B62">
+        <v>185015900000061</v>
+      </c>
+      <c r="C62" t="s">
+        <v>259</v>
+      </c>
+      <c r="D62" t="s">
+        <v>245</v>
+      </c>
+      <c r="E62" t="s">
+        <v>78</v>
+      </c>
+      <c r="F62" s="1">
+        <v>31064</v>
+      </c>
+      <c r="G62" t="s">
+        <v>205</v>
+      </c>
+      <c r="H62">
+        <v>59000</v>
+      </c>
+      <c r="I62" t="s">
+        <v>81</v>
+      </c>
+      <c r="J62" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="63" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A63">
+        <v>62</v>
+      </c>
+      <c r="B63">
+        <v>274065900000062</v>
+      </c>
+      <c r="C63" t="s">
+        <v>260</v>
+      </c>
+      <c r="D63" t="s">
+        <v>246</v>
+      </c>
+      <c r="E63" t="s">
+        <v>79</v>
+      </c>
+      <c r="F63" s="1">
+        <v>27199</v>
+      </c>
+      <c r="G63" t="s">
+        <v>204</v>
+      </c>
+      <c r="H63">
+        <v>59000</v>
+      </c>
+      <c r="I63" t="s">
+        <v>81</v>
+      </c>
+      <c r="J63" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="64" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A64">
+        <v>63</v>
+      </c>
+      <c r="B64">
+        <v>298105900000063</v>
+      </c>
+      <c r="C64" t="s">
+        <v>261</v>
+      </c>
+      <c r="D64" t="s">
+        <v>247</v>
+      </c>
+      <c r="E64" t="s">
+        <v>79</v>
+      </c>
+      <c r="F64" s="1">
+        <v>36078</v>
+      </c>
+      <c r="G64" t="s">
+        <v>206</v>
+      </c>
+      <c r="H64">
+        <v>59000</v>
+      </c>
+      <c r="I64" t="s">
+        <v>81</v>
+      </c>
+      <c r="J64" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="65" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A65">
+        <v>64</v>
+      </c>
+      <c r="B65">
+        <v>191030500000064</v>
+      </c>
+      <c r="C65" t="s">
+        <v>262</v>
+      </c>
+      <c r="D65" t="s">
+        <v>248</v>
+      </c>
+      <c r="E65" t="s">
+        <v>78</v>
+      </c>
+      <c r="F65" s="1">
+        <v>33324</v>
+      </c>
+      <c r="G65" t="s">
+        <v>207</v>
+      </c>
+      <c r="H65">
+        <v>59000</v>
+      </c>
+      <c r="I65" t="s">
+        <v>81</v>
+      </c>
+      <c r="J65" t="s">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="66" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A66">
+        <v>65</v>
+      </c>
+      <c r="B66">
+        <v>183065900000065</v>
+      </c>
+      <c r="C66" t="s">
+        <v>263</v>
+      </c>
+      <c r="D66" t="s">
+        <v>249</v>
+      </c>
+      <c r="E66" t="s">
+        <v>78</v>
+      </c>
+      <c r="F66" s="1">
+        <v>30497</v>
+      </c>
+      <c r="G66" t="s">
+        <v>208</v>
+      </c>
+      <c r="H66">
+        <v>59000</v>
+      </c>
+      <c r="I66" t="s">
+        <v>81</v>
+      </c>
+      <c r="J66" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="67" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A67">
+        <v>66</v>
+      </c>
+      <c r="B67">
+        <v>174025900000066</v>
+      </c>
+      <c r="C67" t="s">
+        <v>264</v>
+      </c>
+      <c r="D67" t="s">
+        <v>67</v>
+      </c>
+      <c r="E67" t="s">
+        <v>78</v>
+      </c>
+      <c r="F67" s="1">
+        <v>27085</v>
+      </c>
+      <c r="G67" t="s">
+        <v>209</v>
+      </c>
+      <c r="H67">
+        <v>59000</v>
+      </c>
+      <c r="I67" t="s">
+        <v>81</v>
+      </c>
+      <c r="J67" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="68" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A68">
+        <v>67</v>
+      </c>
+      <c r="B68">
+        <v>285065900000067</v>
+      </c>
+      <c r="C68" t="s">
+        <v>265</v>
+      </c>
+      <c r="D68" t="s">
+        <v>219</v>
+      </c>
+      <c r="E68" t="s">
+        <v>79</v>
+      </c>
+      <c r="F68" s="1">
+        <v>31211</v>
+      </c>
+      <c r="G68" t="s">
+        <v>210</v>
+      </c>
+      <c r="H68">
+        <v>59000</v>
+      </c>
+      <c r="I68" t="s">
+        <v>81</v>
+      </c>
+      <c r="J68" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="69" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A69">
+        <v>68</v>
+      </c>
+      <c r="B69">
+        <v>266106200000068</v>
+      </c>
+      <c r="C69" t="s">
+        <v>266</v>
+      </c>
+      <c r="D69" t="s">
+        <v>44</v>
+      </c>
+      <c r="E69" t="s">
+        <v>79</v>
+      </c>
+      <c r="F69" s="1">
+        <v>24390</v>
+      </c>
+      <c r="G69" t="s">
+        <v>211</v>
+      </c>
+      <c r="H69">
+        <v>59000</v>
+      </c>
+      <c r="I69" t="s">
+        <v>81</v>
+      </c>
+      <c r="J69" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="70" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A70">
+        <v>69</v>
+      </c>
+      <c r="B70">
+        <v>191085900000069</v>
+      </c>
+      <c r="C70" t="s">
+        <v>267</v>
+      </c>
+      <c r="D70" t="s">
+        <v>42</v>
+      </c>
+      <c r="E70" t="s">
+        <v>78</v>
+      </c>
+      <c r="F70" s="1">
+        <v>33452</v>
+      </c>
+      <c r="G70" t="s">
+        <v>212</v>
+      </c>
+      <c r="H70">
+        <v>59000</v>
+      </c>
+      <c r="I70" t="s">
+        <v>81</v>
+      </c>
+      <c r="J70" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="71" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A71">
+        <v>70</v>
+      </c>
+      <c r="B71">
+        <v>284095900000070</v>
+      </c>
+      <c r="C71" t="s">
+        <v>268</v>
+      </c>
+      <c r="D71" t="s">
+        <v>43</v>
+      </c>
+      <c r="E71" t="s">
+        <v>79</v>
+      </c>
+      <c r="F71" s="1">
+        <v>30951</v>
+      </c>
+      <c r="G71" t="s">
+        <v>213</v>
+      </c>
+      <c r="H71">
+        <v>59000</v>
+      </c>
+      <c r="I71" t="s">
+        <v>81</v>
+      </c>
+      <c r="J71" t="s">
+        <v>184</v>
       </c>
     </row>
   </sheetData>

</xml_diff>